<commit_message>
Se crea la base de datos y se hace el renderizado
</commit_message>
<xml_diff>
--- a/Etapa 01/Diccionario de datos.xlsx
+++ b/Etapa 01/Diccionario de datos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\INA\Proyecto Final\Etapa 01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF472049-8F8C-4815-8090-890482C654F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A8B23B0-2FB5-4900-9BE3-1566B1714BDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19120" yWindow="-80" windowWidth="16960" windowHeight="10060" xr2:uid="{DA776B2A-F68D-4D43-820F-6C5204E56763}"/>
+    <workbookView xWindow="19090" yWindow="-110" windowWidth="17020" windowHeight="10120" xr2:uid="{DA776B2A-F68D-4D43-820F-6C5204E56763}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="68">
   <si>
     <t>Atributo</t>
   </si>
@@ -100,9 +100,6 @@
     <t>Proveedores</t>
   </si>
   <si>
-    <t>ID_REGISTROP</t>
-  </si>
-  <si>
     <t>FK</t>
   </si>
   <si>
@@ -214,9 +211,6 @@
     <t>ID_PRODUCTO</t>
   </si>
   <si>
-    <t>Facturaciones</t>
-  </si>
-  <si>
     <t>ID_FACTURA</t>
   </si>
   <si>
@@ -238,7 +232,13 @@
     <t>ID_DETALLE_FACTURA</t>
   </si>
   <si>
-    <t>Registro_Productos</t>
+    <t>Productos</t>
+  </si>
+  <si>
+    <t>Facturas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INT </t>
   </si>
 </sst>
 </file>
@@ -324,7 +324,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
@@ -348,13 +348,19 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -672,10 +678,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3CAD0CD-A372-4142-AD31-8AE87056CD94}">
-  <dimension ref="E2:L107"/>
+  <dimension ref="E2:L109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D43" sqref="A43:XFD43"/>
+    <sheetView tabSelected="1" topLeftCell="E92" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F93" activeCellId="1" sqref="F106 F93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -686,7 +692,7 @@
   </cols>
   <sheetData>
     <row r="2" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E2" s="13">
+      <c r="E2" s="11">
         <v>1</v>
       </c>
       <c r="F2" s="2"/>
@@ -696,14 +702,14 @@
       <c r="J2" s="2"/>
     </row>
     <row r="3" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E3" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
-      <c r="J3" s="12"/>
+      <c r="E3" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
     </row>
     <row r="4" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E4" s="5" t="s">
@@ -727,7 +733,7 @@
     </row>
     <row r="5" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E5" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F5" s="7" t="s">
         <v>15</v>
@@ -745,7 +751,7 @@
     </row>
     <row r="6" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E6" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F6" s="7" t="s">
         <v>6</v>
@@ -793,7 +799,7 @@
     </row>
     <row r="9" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E9" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F9" s="9" t="s">
         <v>6</v>
@@ -809,7 +815,7 @@
     </row>
     <row r="10" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E10" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F10" s="9" t="s">
         <v>6</v>
@@ -818,14 +824,14 @@
         <v>20</v>
       </c>
       <c r="H10" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
     </row>
     <row r="11" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E11" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F11" s="9" t="s">
         <v>6</v>
@@ -861,20 +867,20 @@
     </row>
     <row r="13" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E13" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G13" s="10"/>
       <c r="H13" s="9" t="s">
         <v>7</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14" spans="5:10" x14ac:dyDescent="0.25">
@@ -895,7 +901,7 @@
     </row>
     <row r="15" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E15" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F15" s="8" t="s">
         <v>6</v>
@@ -933,7 +939,7 @@
       <c r="I18" s="1"/>
     </row>
     <row r="19" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E19" s="13">
+      <c r="E19" s="11">
         <v>2</v>
       </c>
       <c r="F19" s="2"/>
@@ -943,14 +949,14 @@
       <c r="J19" s="2"/>
     </row>
     <row r="20" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E20" s="11" t="s">
+      <c r="E20" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="F20" s="12"/>
-      <c r="G20" s="12"/>
-      <c r="H20" s="12"/>
-      <c r="I20" s="12"/>
-      <c r="J20" s="12"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="15"/>
+      <c r="I20" s="15"/>
+      <c r="J20" s="15"/>
     </row>
     <row r="21" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E21" s="5" t="s">
@@ -974,7 +980,7 @@
     </row>
     <row r="22" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E22" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F22" s="7" t="s">
         <v>15</v>
@@ -992,7 +998,7 @@
     </row>
     <row r="23" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E23" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F23" s="7" t="s">
         <v>6</v>
@@ -1008,7 +1014,7 @@
     </row>
     <row r="24" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E24" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F24" s="7" t="s">
         <v>6</v>
@@ -1017,14 +1023,14 @@
         <v>100</v>
       </c>
       <c r="H24" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
     </row>
     <row r="25" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E25" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F25" s="7" t="s">
         <v>6</v>
@@ -1040,21 +1046,21 @@
     </row>
     <row r="26" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E26" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F26" s="7" t="s">
         <v>15</v>
       </c>
       <c r="G26" s="5"/>
       <c r="H26" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I26" s="3"/>
       <c r="J26" s="3"/>
     </row>
     <row r="27" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E27" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F27" s="9" t="s">
         <v>6</v>
@@ -1063,14 +1069,14 @@
         <v>25</v>
       </c>
       <c r="H27" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I27" s="3"/>
       <c r="J27" s="3"/>
     </row>
     <row r="28" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E28" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F28" s="8" t="s">
         <v>6</v>
@@ -1086,7 +1092,7 @@
     </row>
     <row r="29" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E29" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F29" s="8" t="s">
         <v>6</v>
@@ -1102,7 +1108,7 @@
     </row>
     <row r="30" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E30" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F30" s="8" t="s">
         <v>6</v>
@@ -1117,7 +1123,7 @@
       <c r="J30" s="2"/>
     </row>
     <row r="33" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E33" s="13">
+      <c r="E33" s="11">
         <v>3</v>
       </c>
       <c r="F33" s="2"/>
@@ -1127,14 +1133,14 @@
       <c r="J33" s="2"/>
     </row>
     <row r="34" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E34" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="F34" s="12"/>
-      <c r="G34" s="12"/>
-      <c r="H34" s="12"/>
-      <c r="I34" s="12"/>
-      <c r="J34" s="12"/>
+      <c r="E34" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="F34" s="15"/>
+      <c r="G34" s="15"/>
+      <c r="H34" s="15"/>
+      <c r="I34" s="15"/>
+      <c r="J34" s="15"/>
     </row>
     <row r="35" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E35" s="5" t="s">
@@ -1158,7 +1164,7 @@
     </row>
     <row r="36" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E36" s="3" t="s">
-        <v>21</v>
+        <v>57</v>
       </c>
       <c r="F36" s="7" t="s">
         <v>15</v>
@@ -1176,7 +1182,7 @@
     </row>
     <row r="37" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E37" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F37" s="7" t="s">
         <v>15</v>
@@ -1187,12 +1193,12 @@
       </c>
       <c r="I37" s="2"/>
       <c r="J37" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="38" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E38" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F38" s="7" t="s">
         <v>15</v>
@@ -1203,12 +1209,12 @@
       </c>
       <c r="I38" s="2"/>
       <c r="J38" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="39" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E39" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F39" s="10" t="s">
         <v>6</v>
@@ -1224,7 +1230,7 @@
     </row>
     <row r="40" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E40" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F40" s="9" t="s">
         <v>6</v>
@@ -1240,7 +1246,7 @@
     </row>
     <row r="41" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E41" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F41" s="7" t="s">
         <v>15</v>
@@ -1254,10 +1260,10 @@
     </row>
     <row r="42" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E42" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F42" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G42" s="5">
         <v>8.1999999999999993</v>
@@ -1269,7 +1275,7 @@
       <c r="J42" s="3"/>
     </row>
     <row r="45" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E45" s="13">
+      <c r="E45" s="11">
         <v>4</v>
       </c>
       <c r="F45" s="2"/>
@@ -1279,14 +1285,14 @@
       <c r="J45" s="2"/>
     </row>
     <row r="46" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E46" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="F46" s="12"/>
-      <c r="G46" s="12"/>
-      <c r="H46" s="12"/>
-      <c r="I46" s="12"/>
-      <c r="J46" s="12"/>
+      <c r="E46" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="F46" s="15"/>
+      <c r="G46" s="15"/>
+      <c r="H46" s="15"/>
+      <c r="I46" s="15"/>
+      <c r="J46" s="15"/>
     </row>
     <row r="47" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E47" s="8" t="s">
@@ -1310,7 +1316,7 @@
     </row>
     <row r="48" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E48" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F48" s="7" t="s">
         <v>15</v>
@@ -1328,7 +1334,7 @@
     </row>
     <row r="49" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E49" s="3" t="s">
-        <v>21</v>
+        <v>57</v>
       </c>
       <c r="F49" s="7" t="s">
         <v>15</v>
@@ -1339,110 +1345,116 @@
       </c>
       <c r="I49" s="2"/>
       <c r="J49" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="50" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E50" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="F50" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="G50" s="10"/>
-      <c r="H50" s="9"/>
+        <v>29</v>
+      </c>
+      <c r="F50" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G50" s="8">
+        <v>100</v>
+      </c>
+      <c r="H50" s="7" t="s">
+        <v>7</v>
+      </c>
       <c r="I50" s="2"/>
       <c r="J50" s="2"/>
     </row>
     <row r="51" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E51" s="3" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="F51" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="G51" s="8">
-        <v>100</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="G51" s="8"/>
       <c r="H51" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I51" s="2"/>
-      <c r="J51" s="2"/>
+      <c r="I51" s="3"/>
+      <c r="J51" s="3"/>
     </row>
     <row r="52" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E52" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="F52" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="G52" s="8"/>
-      <c r="H52" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="I52" s="3"/>
-      <c r="J52" s="3"/>
-    </row>
-    <row r="53" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E53" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F53" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="G53" s="8">
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="H53" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="I53" s="2"/>
-      <c r="J53" s="2"/>
+      <c r="E52" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F52" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="G52" s="8">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="H52" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="I52" s="2"/>
+      <c r="J52" s="2"/>
+    </row>
+    <row r="55" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E55" s="11">
+        <v>5</v>
+      </c>
+      <c r="F55" s="2"/>
+      <c r="G55" s="2"/>
+      <c r="H55" s="2"/>
+      <c r="I55" s="2"/>
+      <c r="J55" s="2"/>
     </row>
     <row r="56" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E56" s="13">
+      <c r="E56" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="F56" s="15"/>
+      <c r="G56" s="15"/>
+      <c r="H56" s="15"/>
+      <c r="I56" s="15"/>
+      <c r="J56" s="15"/>
+    </row>
+    <row r="57" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E57" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="F57" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="G57" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="H57" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="I57" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J57" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="F56" s="2"/>
-      <c r="G56" s="2"/>
-      <c r="H56" s="2"/>
-      <c r="I56" s="2"/>
-      <c r="J56" s="2"/>
-    </row>
-    <row r="57" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E57" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="F57" s="12"/>
-      <c r="G57" s="12"/>
-      <c r="H57" s="12"/>
-      <c r="I57" s="12"/>
-      <c r="J57" s="12"/>
     </row>
     <row r="58" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E58" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="F58" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="G58" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="H58" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="I58" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="J58" s="8" t="s">
-        <v>5</v>
+      <c r="E58" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F58" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G58" s="8"/>
+      <c r="H58" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I58" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J58" s="3" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="59" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E59" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F59" s="7" t="s">
         <v>15</v>
@@ -1451,87 +1463,85 @@
       <c r="H59" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I59" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="J59" s="3" t="s">
-        <v>8</v>
+      <c r="I59" s="2"/>
+      <c r="J59" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="60" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E60" s="3" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="F60" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="G60" s="8"/>
+        <v>6</v>
+      </c>
+      <c r="G60" s="8">
+        <v>50</v>
+      </c>
       <c r="H60" s="7" t="s">
         <v>7</v>
       </c>
       <c r="I60" s="2"/>
       <c r="J60" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="61" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E61" s="3" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F61" s="7" t="s">
         <v>6</v>
       </c>
       <c r="G61" s="8">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="H61" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I61" s="2"/>
-      <c r="J61" s="2" t="s">
+      <c r="I61" s="3"/>
+      <c r="J61" s="3"/>
+    </row>
+    <row r="62" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E62" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="62" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E62" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F62" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="G62" s="8">
-        <v>100</v>
-      </c>
-      <c r="H62" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="I62" s="3"/>
-      <c r="J62" s="3"/>
+      <c r="F62" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G62" s="8"/>
+      <c r="H62" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="I62" s="2"/>
+      <c r="J62" s="2"/>
+      <c r="L62" s="1"/>
     </row>
     <row r="63" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E63" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F63" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F63" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="G63" s="8"/>
+      <c r="G63" s="8">
+        <v>10.199999999999999</v>
+      </c>
       <c r="H63" s="8" t="s">
         <v>7</v>
       </c>
       <c r="I63" s="2"/>
       <c r="J63" s="2"/>
-      <c r="L63" s="1"/>
     </row>
     <row r="64" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E64" s="2" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="F64" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G64" s="8">
-        <v>8.1999999999999993</v>
+        <v>10.199999999999999</v>
       </c>
       <c r="H64" s="8" t="s">
         <v>7</v>
@@ -1541,109 +1551,109 @@
     </row>
     <row r="65" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E65" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="F65" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="G65" s="8">
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="H65" s="8" t="s">
-        <v>7</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="F65" s="8">
+        <v>4.2</v>
+      </c>
+      <c r="G65" s="8"/>
+      <c r="H65" s="8"/>
       <c r="I65" s="2"/>
       <c r="J65" s="2"/>
     </row>
     <row r="66" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E66" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="F66" s="8">
-        <v>4.2</v>
-      </c>
-      <c r="G66" s="8"/>
-      <c r="H66" s="8"/>
+        <v>61</v>
+      </c>
+      <c r="F66" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="G66" s="10">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="H66" s="10" t="s">
+        <v>7</v>
+      </c>
       <c r="I66" s="2"/>
       <c r="J66" s="2"/>
     </row>
-    <row r="67" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E67" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="F67" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="G67" s="10">
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="H67" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="I67" s="2"/>
-      <c r="J67" s="2"/>
+    <row r="69" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E69" s="11">
+        <v>6</v>
+      </c>
+      <c r="F69" s="2"/>
+      <c r="G69" s="2"/>
+      <c r="H69" s="2"/>
+      <c r="I69" s="2"/>
+      <c r="J69" s="2"/>
     </row>
     <row r="70" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E70" s="13">
-        <v>6</v>
-      </c>
-      <c r="F70" s="2"/>
-      <c r="G70" s="2"/>
-      <c r="H70" s="2"/>
-      <c r="I70" s="2"/>
-      <c r="J70" s="2"/>
+      <c r="E70" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="F70" s="15"/>
+      <c r="G70" s="15"/>
+      <c r="H70" s="15"/>
+      <c r="I70" s="15"/>
+      <c r="J70" s="15"/>
     </row>
     <row r="71" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E71" s="11" t="s">
+      <c r="E71" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="F71" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="G71" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="H71" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="I71" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J71" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="72" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E72" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="F71" s="12"/>
-      <c r="G71" s="12"/>
-      <c r="H71" s="12"/>
-      <c r="I71" s="12"/>
-      <c r="J71" s="12"/>
-    </row>
-    <row r="72" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E72" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="F72" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="G72" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="H72" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="I72" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="J72" s="8" t="s">
-        <v>5</v>
+      <c r="F72" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G72" s="8"/>
+      <c r="H72" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I72" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J72" s="3" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="73" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E73" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="F73" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="G73" s="8"/>
-      <c r="H73" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="I73" s="3" t="s">
-        <v>16</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="F73" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="G73" s="13"/>
+      <c r="H73" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="I73" s="3"/>
       <c r="J73" s="3" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
     </row>
     <row r="74" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E74" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F74" s="9" t="s">
         <v>6</v>
@@ -1652,14 +1662,14 @@
         <v>20</v>
       </c>
       <c r="H74" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I74" s="3"/>
       <c r="J74" s="3"/>
     </row>
     <row r="75" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E75" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F75" s="7" t="s">
         <v>6</v>
@@ -1675,7 +1685,7 @@
     </row>
     <row r="76" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E76" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F76" s="7" t="s">
         <v>6</v>
@@ -1691,7 +1701,7 @@
     </row>
     <row r="77" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E77" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F77" s="7" t="s">
         <v>6</v>
@@ -1707,7 +1717,7 @@
     </row>
     <row r="78" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E78" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F78" s="8" t="s">
         <v>6</v>
@@ -1723,7 +1733,7 @@
     </row>
     <row r="79" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E79" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F79" s="8" t="s">
         <v>6</v>
@@ -1732,7 +1742,7 @@
         <v>100</v>
       </c>
       <c r="H79" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I79" s="2"/>
       <c r="J79" s="2"/>
@@ -1746,7 +1756,7 @@
       <c r="J80" s="2"/>
     </row>
     <row r="83" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E83" s="13">
+      <c r="E83" s="11">
         <v>7</v>
       </c>
       <c r="F83" s="2"/>
@@ -1756,14 +1766,14 @@
       <c r="J83" s="2"/>
     </row>
     <row r="84" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E84" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="F84" s="12"/>
-      <c r="G84" s="12"/>
-      <c r="H84" s="12"/>
-      <c r="I84" s="12"/>
-      <c r="J84" s="12"/>
+      <c r="E84" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="F84" s="15"/>
+      <c r="G84" s="15"/>
+      <c r="H84" s="15"/>
+      <c r="I84" s="15"/>
+      <c r="J84" s="15"/>
     </row>
     <row r="85" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E85" s="8" t="s">
@@ -1787,7 +1797,7 @@
     </row>
     <row r="86" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E86" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F86" s="7" t="s">
         <v>15</v>
@@ -1805,169 +1815,177 @@
     </row>
     <row r="87" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E87" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="F87" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="G87" s="8"/>
-      <c r="H87" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="I87" s="2"/>
-      <c r="J87" s="2" t="s">
-        <v>22</v>
+        <v>58</v>
+      </c>
+      <c r="F87" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="G87" s="13"/>
+      <c r="H87" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="I87" s="3"/>
+      <c r="J87" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="88" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E88" s="3" t="s">
-        <v>37</v>
+        <v>59</v>
       </c>
       <c r="F88" s="7" t="s">
-        <v>38</v>
+        <v>15</v>
       </c>
       <c r="G88" s="8"/>
       <c r="H88" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I88" s="2" t="s">
-        <v>48</v>
-      </c>
+      <c r="I88" s="2"/>
       <c r="J88" s="2" t="s">
-        <v>49</v>
+        <v>21</v>
       </c>
     </row>
     <row r="89" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E89" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F89" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="G89" s="13">
         <v>50</v>
       </c>
-      <c r="F89" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="G89" s="8"/>
-      <c r="H89" s="7" t="s">
+      <c r="H89" s="12" t="s">
         <v>7</v>
       </c>
       <c r="I89" s="2"/>
-      <c r="J89" s="2"/>
+      <c r="J89" s="2" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="90" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E90" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="F90" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G90" s="8">
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="H90" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="I90" s="3"/>
-      <c r="J90" s="3"/>
+        <v>29</v>
+      </c>
+      <c r="F90" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="G90" s="13">
+        <v>100</v>
+      </c>
+      <c r="H90" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="I90" s="2"/>
+      <c r="J90" s="2"/>
     </row>
     <row r="91" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E91" s="2"/>
-      <c r="F91" s="2"/>
+      <c r="E91" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F91" s="7" t="s">
+        <v>37</v>
+      </c>
       <c r="G91" s="8"/>
-      <c r="H91" s="8"/>
-      <c r="I91" s="2"/>
-      <c r="J91" s="2"/>
+      <c r="H91" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I91" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="J91" s="2" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="92" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E92" s="2"/>
-      <c r="F92" s="2"/>
+      <c r="E92" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F92" s="7" t="s">
+        <v>15</v>
+      </c>
       <c r="G92" s="8"/>
-      <c r="H92" s="8"/>
+      <c r="H92" s="7" t="s">
+        <v>7</v>
+      </c>
       <c r="I92" s="2"/>
       <c r="J92" s="2"/>
     </row>
     <row r="93" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E93" s="2"/>
-      <c r="F93" s="2"/>
-      <c r="G93" s="8"/>
-      <c r="H93" s="8"/>
+      <c r="E93" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F93" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="G93" s="8">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="H93" s="8" t="s">
+        <v>7</v>
+      </c>
       <c r="I93" s="2"/>
       <c r="J93" s="2"/>
     </row>
-    <row r="96" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E96" s="13">
+    <row r="94" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E94" s="2"/>
+      <c r="F94" s="2"/>
+      <c r="G94" s="8"/>
+      <c r="H94" s="8"/>
+      <c r="I94" s="2"/>
+      <c r="J94" s="2"/>
+    </row>
+    <row r="95" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E95" s="2"/>
+      <c r="F95" s="2"/>
+      <c r="G95" s="8"/>
+      <c r="H95" s="8"/>
+      <c r="I95" s="2"/>
+      <c r="J95" s="2"/>
+    </row>
+    <row r="98" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E98" s="11">
         <v>8</v>
       </c>
-      <c r="F96" s="2"/>
-      <c r="G96" s="2"/>
-      <c r="H96" s="2"/>
-      <c r="I96" s="2"/>
-      <c r="J96" s="2"/>
-    </row>
-    <row r="97" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E97" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="F97" s="12"/>
-      <c r="G97" s="12"/>
-      <c r="H97" s="12"/>
-      <c r="I97" s="12"/>
-      <c r="J97" s="12"/>
-    </row>
-    <row r="98" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E98" s="10" t="s">
+      <c r="F98" s="2"/>
+      <c r="G98" s="2"/>
+      <c r="H98" s="2"/>
+      <c r="I98" s="2"/>
+      <c r="J98" s="2"/>
+    </row>
+    <row r="99" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E99" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="F99" s="15"/>
+      <c r="G99" s="15"/>
+      <c r="H99" s="15"/>
+      <c r="I99" s="15"/>
+      <c r="J99" s="15"/>
+    </row>
+    <row r="100" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E100" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="F98" s="10" t="s">
+      <c r="F100" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="G98" s="10" t="s">
+      <c r="G100" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="H98" s="10" t="s">
+      <c r="H100" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="I98" s="10" t="s">
+      <c r="I100" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="J98" s="10" t="s">
+      <c r="J100" s="10" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="99" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E99" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="F99" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="G99" s="10"/>
-      <c r="H99" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="I99" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="J99" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="100" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E100" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="F100" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="G100" s="10"/>
-      <c r="H100" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="I100" s="2"/>
-      <c r="J100" s="2" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="101" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E101" s="3" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="F101" s="9" t="s">
         <v>15</v>
@@ -1976,30 +1994,32 @@
       <c r="H101" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="I101" s="2"/>
-      <c r="J101" s="2"/>
+      <c r="I101" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J101" s="3" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="102" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E102" s="3" t="s">
-        <v>37</v>
+        <v>58</v>
       </c>
       <c r="F102" s="9" t="s">
-        <v>38</v>
+        <v>15</v>
       </c>
       <c r="G102" s="10"/>
       <c r="H102" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="I102" s="2" t="s">
-        <v>48</v>
-      </c>
+      <c r="I102" s="2"/>
       <c r="J102" s="2" t="s">
-        <v>49</v>
+        <v>21</v>
       </c>
     </row>
     <row r="103" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E103" s="3" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="F103" s="9" t="s">
         <v>15</v>
@@ -2013,35 +2033,51 @@
     </row>
     <row r="104" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E104" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="F104" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G104" s="10">
-        <v>8.1999999999999993</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="F104" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="G104" s="10"/>
       <c r="H104" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="I104" s="3"/>
-      <c r="J104" s="3"/>
+      <c r="I104" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="J104" s="2" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="105" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E105" s="2"/>
-      <c r="F105" s="2"/>
+      <c r="E105" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F105" s="9" t="s">
+        <v>15</v>
+      </c>
       <c r="G105" s="10"/>
-      <c r="H105" s="10"/>
+      <c r="H105" s="9" t="s">
+        <v>7</v>
+      </c>
       <c r="I105" s="2"/>
       <c r="J105" s="2"/>
     </row>
     <row r="106" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E106" s="2"/>
-      <c r="F106" s="2"/>
-      <c r="G106" s="10"/>
-      <c r="H106" s="10"/>
-      <c r="I106" s="2"/>
-      <c r="J106" s="2"/>
+      <c r="E106" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F106" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="G106" s="10">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="H106" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="I106" s="3"/>
+      <c r="J106" s="3"/>
     </row>
     <row r="107" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E107" s="2"/>
@@ -2051,16 +2087,32 @@
       <c r="I107" s="2"/>
       <c r="J107" s="2"/>
     </row>
+    <row r="108" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E108" s="2"/>
+      <c r="F108" s="2"/>
+      <c r="G108" s="10"/>
+      <c r="H108" s="10"/>
+      <c r="I108" s="2"/>
+      <c r="J108" s="2"/>
+    </row>
+    <row r="109" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E109" s="2"/>
+      <c r="F109" s="2"/>
+      <c r="G109" s="10"/>
+      <c r="H109" s="10"/>
+      <c r="I109" s="2"/>
+      <c r="J109" s="2"/>
+    </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="E97:J97"/>
-    <mergeCell ref="E71:J71"/>
+    <mergeCell ref="E99:J99"/>
+    <mergeCell ref="E70:J70"/>
     <mergeCell ref="E84:J84"/>
     <mergeCell ref="E3:J3"/>
     <mergeCell ref="E20:J20"/>
     <mergeCell ref="E34:J34"/>
     <mergeCell ref="E46:J46"/>
-    <mergeCell ref="E57:J57"/>
+    <mergeCell ref="E56:J56"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>

<commit_message>
Se realizan pruebas en la base de datos ingresando datos
</commit_message>
<xml_diff>
--- a/Etapa 01/Diccionario de datos.xlsx
+++ b/Etapa 01/Diccionario de datos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\INA\Proyecto Final\Etapa 01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A8B23B0-2FB5-4900-9BE3-1566B1714BDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB47D8A7-37F2-4795-ADA5-318770070868}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19090" yWindow="-110" windowWidth="17020" windowHeight="10120" xr2:uid="{DA776B2A-F68D-4D43-820F-6C5204E56763}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="68">
   <si>
     <t>Atributo</t>
   </si>
@@ -678,10 +678,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3CAD0CD-A372-4142-AD31-8AE87056CD94}">
-  <dimension ref="E2:L109"/>
+  <dimension ref="E2:L108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E92" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F93" activeCellId="1" sqref="F106 F93"/>
+    <sheetView tabSelected="1" topLeftCell="E32" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1182,7 +1182,7 @@
     </row>
     <row r="37" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E37" s="3" t="s">
-        <v>59</v>
+        <v>24</v>
       </c>
       <c r="F37" s="7" t="s">
         <v>15</v>
@@ -1197,32 +1197,32 @@
       </c>
     </row>
     <row r="38" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E38" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F38" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="G38" s="5"/>
-      <c r="H38" s="6" t="s">
+      <c r="E38" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F38" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="G38" s="10">
+        <v>50</v>
+      </c>
+      <c r="H38" s="10" t="s">
         <v>7</v>
       </c>
       <c r="I38" s="2"/>
-      <c r="J38" s="2" t="s">
-        <v>21</v>
-      </c>
+      <c r="J38" s="2"/>
     </row>
     <row r="39" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E39" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="F39" s="10" t="s">
+      <c r="E39" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F39" s="9" t="s">
         <v>6</v>
       </c>
       <c r="G39" s="10">
-        <v>50</v>
-      </c>
-      <c r="H39" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="H39" s="9" t="s">
         <v>7</v>
       </c>
       <c r="I39" s="2"/>
@@ -1230,15 +1230,13 @@
     </row>
     <row r="40" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E40" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="F40" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="G40" s="10">
-        <v>100</v>
-      </c>
-      <c r="H40" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F40" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G40" s="5"/>
+      <c r="H40" s="6" t="s">
         <v>7</v>
       </c>
       <c r="I40" s="2"/>
@@ -1246,77 +1244,81 @@
     </row>
     <row r="41" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E41" s="3" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="F41" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G41" s="5">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="H41" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="I41" s="3"/>
+      <c r="J41" s="3"/>
+    </row>
+    <row r="44" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E44" s="11">
+        <v>4</v>
+      </c>
+      <c r="F44" s="2"/>
+      <c r="G44" s="2"/>
+      <c r="H44" s="2"/>
+      <c r="I44" s="2"/>
+      <c r="J44" s="2"/>
+    </row>
+    <row r="45" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E45" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="F45" s="15"/>
+      <c r="G45" s="15"/>
+      <c r="H45" s="15"/>
+      <c r="I45" s="15"/>
+      <c r="J45" s="15"/>
+    </row>
+    <row r="46" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E46" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="F46" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="G46" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="H46" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="I46" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J46" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="47" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E47" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F47" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="G41" s="5"/>
-      <c r="H41" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="I41" s="2"/>
-      <c r="J41" s="2"/>
-    </row>
-    <row r="42" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E42" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="F42" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="G42" s="5">
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="H42" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="I42" s="3"/>
-      <c r="J42" s="3"/>
-    </row>
-    <row r="45" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E45" s="11">
-        <v>4</v>
-      </c>
-      <c r="F45" s="2"/>
-      <c r="G45" s="2"/>
-      <c r="H45" s="2"/>
-      <c r="I45" s="2"/>
-      <c r="J45" s="2"/>
-    </row>
-    <row r="46" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E46" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="F46" s="15"/>
-      <c r="G46" s="15"/>
-      <c r="H46" s="15"/>
-      <c r="I46" s="15"/>
-      <c r="J46" s="15"/>
-    </row>
-    <row r="47" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E47" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="F47" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="G47" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="H47" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="I47" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="J47" s="8" t="s">
-        <v>5</v>
+      <c r="G47" s="8"/>
+      <c r="H47" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I47" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J47" s="3" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="48" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E48" s="3" t="s">
-        <v>34</v>
+        <v>57</v>
       </c>
       <c r="F48" s="7" t="s">
         <v>15</v>
@@ -1325,118 +1327,118 @@
       <c r="H48" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I48" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="J48" s="3" t="s">
-        <v>8</v>
+      <c r="I48" s="2"/>
+      <c r="J48" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="49" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E49" s="3" t="s">
-        <v>57</v>
+        <v>29</v>
       </c>
       <c r="F49" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="G49" s="8"/>
+        <v>6</v>
+      </c>
+      <c r="G49" s="8">
+        <v>100</v>
+      </c>
       <c r="H49" s="7" t="s">
         <v>7</v>
       </c>
       <c r="I49" s="2"/>
-      <c r="J49" s="2" t="s">
-        <v>21</v>
-      </c>
+      <c r="J49" s="2"/>
     </row>
     <row r="50" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E50" s="3" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="F50" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="G50" s="8">
-        <v>100</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="G50" s="8"/>
       <c r="H50" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I50" s="2"/>
-      <c r="J50" s="2"/>
+      <c r="I50" s="3"/>
+      <c r="J50" s="3"/>
     </row>
     <row r="51" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E51" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="F51" s="7" t="s">
+      <c r="E51" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F51" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="G51" s="8">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="H51" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="I51" s="2"/>
+      <c r="J51" s="2"/>
+    </row>
+    <row r="54" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E54" s="11">
+        <v>5</v>
+      </c>
+      <c r="F54" s="2"/>
+      <c r="G54" s="2"/>
+      <c r="H54" s="2"/>
+      <c r="I54" s="2"/>
+      <c r="J54" s="2"/>
+    </row>
+    <row r="55" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E55" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="F55" s="15"/>
+      <c r="G55" s="15"/>
+      <c r="H55" s="15"/>
+      <c r="I55" s="15"/>
+      <c r="J55" s="15"/>
+    </row>
+    <row r="56" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E56" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="F56" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="G56" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="H56" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="I56" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J56" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="57" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E57" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F57" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="G51" s="8"/>
-      <c r="H51" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="I51" s="3"/>
-      <c r="J51" s="3"/>
-    </row>
-    <row r="52" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E52" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="F52" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="G52" s="8">
-        <v>10.199999999999999</v>
-      </c>
-      <c r="H52" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="I52" s="2"/>
-      <c r="J52" s="2"/>
-    </row>
-    <row r="55" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E55" s="11">
-        <v>5</v>
-      </c>
-      <c r="F55" s="2"/>
-      <c r="G55" s="2"/>
-      <c r="H55" s="2"/>
-      <c r="I55" s="2"/>
-      <c r="J55" s="2"/>
-    </row>
-    <row r="56" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E56" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="F56" s="15"/>
-      <c r="G56" s="15"/>
-      <c r="H56" s="15"/>
-      <c r="I56" s="15"/>
-      <c r="J56" s="15"/>
-    </row>
-    <row r="57" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E57" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="F57" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="G57" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="H57" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="I57" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="J57" s="8" t="s">
-        <v>5</v>
+      <c r="G57" s="8"/>
+      <c r="H57" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I57" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J57" s="3" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="58" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E58" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F58" s="7" t="s">
         <v>15</v>
@@ -1445,21 +1447,21 @@
       <c r="H58" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I58" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="J58" s="3" t="s">
-        <v>8</v>
+      <c r="I58" s="2"/>
+      <c r="J58" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="59" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E59" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F59" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="G59" s="8"/>
+        <v>6</v>
+      </c>
+      <c r="G59" s="8">
+        <v>50</v>
+      </c>
       <c r="H59" s="7" t="s">
         <v>7</v>
       </c>
@@ -1470,56 +1472,54 @@
     </row>
     <row r="60" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E60" s="3" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="F60" s="7" t="s">
         <v>6</v>
       </c>
       <c r="G60" s="8">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="H60" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I60" s="2"/>
-      <c r="J60" s="2" t="s">
-        <v>21</v>
-      </c>
+      <c r="I60" s="3"/>
+      <c r="J60" s="3"/>
     </row>
     <row r="61" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E61" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="F61" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="G61" s="8">
-        <v>100</v>
-      </c>
-      <c r="H61" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="I61" s="3"/>
-      <c r="J61" s="3"/>
+      <c r="E61" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F61" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G61" s="8"/>
+      <c r="H61" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="I61" s="2"/>
+      <c r="J61" s="2"/>
+      <c r="L61" s="1"/>
     </row>
     <row r="62" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E62" s="2" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="F62" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="G62" s="8"/>
+        <v>23</v>
+      </c>
+      <c r="G62" s="8">
+        <v>10.199999999999999</v>
+      </c>
       <c r="H62" s="8" t="s">
         <v>7</v>
       </c>
       <c r="I62" s="2"/>
       <c r="J62" s="2"/>
-      <c r="L62" s="1"/>
     </row>
     <row r="63" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E63" s="2" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="F63" s="8" t="s">
         <v>23</v>
@@ -1535,141 +1535,141 @@
     </row>
     <row r="64" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E64" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F64" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="G64" s="8">
-        <v>10.199999999999999</v>
-      </c>
-      <c r="H64" s="8" t="s">
-        <v>7</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="F64" s="8">
+        <v>4.2</v>
+      </c>
+      <c r="G64" s="8"/>
+      <c r="H64" s="8"/>
       <c r="I64" s="2"/>
       <c r="J64" s="2"/>
     </row>
     <row r="65" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E65" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F65" s="8">
-        <v>4.2</v>
-      </c>
-      <c r="G65" s="8"/>
-      <c r="H65" s="8"/>
+        <v>61</v>
+      </c>
+      <c r="F65" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="G65" s="10">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="H65" s="10" t="s">
+        <v>7</v>
+      </c>
       <c r="I65" s="2"/>
       <c r="J65" s="2"/>
     </row>
-    <row r="66" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E66" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="F66" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="G66" s="10">
-        <v>10.199999999999999</v>
-      </c>
-      <c r="H66" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="I66" s="2"/>
-      <c r="J66" s="2"/>
+    <row r="68" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E68" s="11">
+        <v>6</v>
+      </c>
+      <c r="F68" s="2"/>
+      <c r="G68" s="2"/>
+      <c r="H68" s="2"/>
+      <c r="I68" s="2"/>
+      <c r="J68" s="2"/>
     </row>
     <row r="69" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E69" s="11">
-        <v>6</v>
-      </c>
-      <c r="F69" s="2"/>
-      <c r="G69" s="2"/>
-      <c r="H69" s="2"/>
-      <c r="I69" s="2"/>
-      <c r="J69" s="2"/>
+      <c r="E69" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="F69" s="15"/>
+      <c r="G69" s="15"/>
+      <c r="H69" s="15"/>
+      <c r="I69" s="15"/>
+      <c r="J69" s="15"/>
     </row>
     <row r="70" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E70" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="F70" s="15"/>
-      <c r="G70" s="15"/>
-      <c r="H70" s="15"/>
-      <c r="I70" s="15"/>
-      <c r="J70" s="15"/>
+      <c r="E70" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="F70" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="G70" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="H70" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="I70" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J70" s="8" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="71" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E71" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="F71" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="G71" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="H71" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="I71" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="J71" s="8" t="s">
-        <v>5</v>
+      <c r="E71" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F71" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G71" s="8"/>
+      <c r="H71" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I71" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J71" s="3" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="72" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E72" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="F72" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="F72" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="G72" s="8"/>
-      <c r="H72" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="I72" s="3" t="s">
-        <v>16</v>
-      </c>
+      <c r="G72" s="13"/>
+      <c r="H72" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="I72" s="3"/>
       <c r="J72" s="3" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
     </row>
     <row r="73" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E73" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="F73" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="G73" s="13"/>
-      <c r="H73" s="12" t="s">
-        <v>7</v>
+        <v>62</v>
+      </c>
+      <c r="F73" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="G73" s="10">
+        <v>20</v>
+      </c>
+      <c r="H73" s="9" t="s">
+        <v>54</v>
       </c>
       <c r="I73" s="3"/>
-      <c r="J73" s="3" t="s">
-        <v>21</v>
-      </c>
+      <c r="J73" s="3"/>
     </row>
     <row r="74" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E74" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F74" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="G74" s="10">
+        <v>42</v>
+      </c>
+      <c r="F74" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G74" s="8">
         <v>20</v>
       </c>
-      <c r="H74" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="I74" s="3"/>
-      <c r="J74" s="3"/>
+      <c r="H74" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I74" s="2"/>
+      <c r="J74" s="2"/>
     </row>
     <row r="75" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E75" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F75" s="7" t="s">
         <v>6</v>
@@ -1685,7 +1685,7 @@
     </row>
     <row r="76" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E76" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F76" s="7" t="s">
         <v>6</v>
@@ -1696,148 +1696,150 @@
       <c r="H76" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I76" s="2"/>
-      <c r="J76" s="2"/>
+      <c r="I76" s="3"/>
+      <c r="J76" s="3"/>
     </row>
     <row r="77" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E77" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="F77" s="7" t="s">
+      <c r="E77" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F77" s="8" t="s">
         <v>6</v>
       </c>
       <c r="G77" s="8">
         <v>20</v>
       </c>
-      <c r="H77" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="I77" s="3"/>
-      <c r="J77" s="3"/>
+      <c r="H77" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="I77" s="2"/>
+      <c r="J77" s="2"/>
     </row>
     <row r="78" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E78" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F78" s="8" t="s">
         <v>6</v>
       </c>
       <c r="G78" s="8">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="H78" s="8" t="s">
-        <v>7</v>
+        <v>54</v>
       </c>
       <c r="I78" s="2"/>
       <c r="J78" s="2"/>
     </row>
     <row r="79" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E79" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F79" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="G79" s="8">
-        <v>100</v>
-      </c>
-      <c r="H79" s="8" t="s">
-        <v>54</v>
-      </c>
+      <c r="E79" s="2"/>
+      <c r="F79" s="2"/>
+      <c r="G79" s="8"/>
+      <c r="H79" s="8"/>
       <c r="I79" s="2"/>
       <c r="J79" s="2"/>
     </row>
-    <row r="80" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E80" s="2"/>
-      <c r="F80" s="2"/>
-      <c r="G80" s="8"/>
-      <c r="H80" s="8"/>
-      <c r="I80" s="2"/>
-      <c r="J80" s="2"/>
+    <row r="82" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E82" s="11">
+        <v>7</v>
+      </c>
+      <c r="F82" s="2"/>
+      <c r="G82" s="2"/>
+      <c r="H82" s="2"/>
+      <c r="I82" s="2"/>
+      <c r="J82" s="2"/>
     </row>
     <row r="83" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E83" s="11">
-        <v>7</v>
-      </c>
-      <c r="F83" s="2"/>
-      <c r="G83" s="2"/>
-      <c r="H83" s="2"/>
-      <c r="I83" s="2"/>
-      <c r="J83" s="2"/>
+      <c r="E83" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="F83" s="15"/>
+      <c r="G83" s="15"/>
+      <c r="H83" s="15"/>
+      <c r="I83" s="15"/>
+      <c r="J83" s="15"/>
     </row>
     <row r="84" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E84" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="F84" s="15"/>
-      <c r="G84" s="15"/>
-      <c r="H84" s="15"/>
-      <c r="I84" s="15"/>
-      <c r="J84" s="15"/>
+      <c r="E84" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="F84" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="G84" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="H84" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="I84" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J84" s="8" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="85" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E85" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="F85" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="G85" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="H85" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="I85" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="J85" s="8" t="s">
-        <v>5</v>
+      <c r="E85" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F85" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G85" s="8"/>
+      <c r="H85" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I85" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J85" s="3" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="86" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E86" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="F86" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="G86" s="8"/>
-      <c r="H86" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="I86" s="3" t="s">
-        <v>16</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="F86" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="G86" s="13"/>
+      <c r="H86" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="I86" s="3"/>
       <c r="J86" s="3" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
     </row>
     <row r="87" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E87" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="F87" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="G87" s="13"/>
-      <c r="H87" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="I87" s="3"/>
-      <c r="J87" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F87" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G87" s="8"/>
+      <c r="H87" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I87" s="2"/>
+      <c r="J87" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="88" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E88" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="F88" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="G88" s="8"/>
-      <c r="H88" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="F88" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="G88" s="13">
+        <v>50</v>
+      </c>
+      <c r="H88" s="12" t="s">
         <v>7</v>
       </c>
       <c r="I88" s="2"/>
@@ -1847,83 +1849,73 @@
     </row>
     <row r="89" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E89" s="3" t="s">
-        <v>57</v>
+        <v>29</v>
       </c>
       <c r="F89" s="12" t="s">
         <v>6</v>
       </c>
       <c r="G89" s="13">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="H89" s="12" t="s">
         <v>7</v>
       </c>
       <c r="I89" s="2"/>
-      <c r="J89" s="2" t="s">
-        <v>21</v>
-      </c>
+      <c r="J89" s="2"/>
     </row>
     <row r="90" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E90" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="F90" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="G90" s="13">
-        <v>100</v>
-      </c>
-      <c r="H90" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="I90" s="2"/>
-      <c r="J90" s="2"/>
+        <v>36</v>
+      </c>
+      <c r="F90" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="G90" s="8"/>
+      <c r="H90" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I90" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="J90" s="2" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="91" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E91" s="3" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="F91" s="7" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="G91" s="8"/>
       <c r="H91" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I91" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="J91" s="2" t="s">
-        <v>48</v>
-      </c>
+      <c r="I91" s="2"/>
+      <c r="J91" s="2"/>
     </row>
     <row r="92" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E92" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F92" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="G92" s="8"/>
-      <c r="H92" s="7" t="s">
+      <c r="E92" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F92" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="G92" s="8">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="H92" s="8" t="s">
         <v>7</v>
       </c>
       <c r="I92" s="2"/>
       <c r="J92" s="2"/>
     </row>
     <row r="93" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E93" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="F93" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="G93" s="8">
-        <v>10.199999999999999</v>
-      </c>
-      <c r="H93" s="8" t="s">
-        <v>7</v>
-      </c>
+      <c r="E93" s="2"/>
+      <c r="F93" s="2"/>
+      <c r="G93" s="8"/>
+      <c r="H93" s="8"/>
       <c r="I93" s="2"/>
       <c r="J93" s="2"/>
     </row>
@@ -1935,57 +1927,67 @@
       <c r="I94" s="2"/>
       <c r="J94" s="2"/>
     </row>
-    <row r="95" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E95" s="2"/>
-      <c r="F95" s="2"/>
-      <c r="G95" s="8"/>
-      <c r="H95" s="8"/>
-      <c r="I95" s="2"/>
-      <c r="J95" s="2"/>
+    <row r="97" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E97" s="11">
+        <v>8</v>
+      </c>
+      <c r="F97" s="2"/>
+      <c r="G97" s="2"/>
+      <c r="H97" s="2"/>
+      <c r="I97" s="2"/>
+      <c r="J97" s="2"/>
     </row>
     <row r="98" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E98" s="11">
+      <c r="E98" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="F98" s="15"/>
+      <c r="G98" s="15"/>
+      <c r="H98" s="15"/>
+      <c r="I98" s="15"/>
+      <c r="J98" s="15"/>
+    </row>
+    <row r="99" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E99" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="F99" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="G99" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="H99" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="I99" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="J99" s="10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="100" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E100" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F100" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G100" s="10"/>
+      <c r="H100" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="I100" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J100" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="F98" s="2"/>
-      <c r="G98" s="2"/>
-      <c r="H98" s="2"/>
-      <c r="I98" s="2"/>
-      <c r="J98" s="2"/>
-    </row>
-    <row r="99" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E99" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="F99" s="15"/>
-      <c r="G99" s="15"/>
-      <c r="H99" s="15"/>
-      <c r="I99" s="15"/>
-      <c r="J99" s="15"/>
-    </row>
-    <row r="100" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E100" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="F100" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="G100" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="H100" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="I100" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="J100" s="10" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="101" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E101" s="3" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="F101" s="9" t="s">
         <v>15</v>
@@ -1994,16 +1996,14 @@
       <c r="H101" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="I101" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="J101" s="3" t="s">
-        <v>8</v>
+      <c r="I101" s="2"/>
+      <c r="J101" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="102" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E102" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F102" s="9" t="s">
         <v>15</v>
@@ -2013,71 +2013,63 @@
         <v>7</v>
       </c>
       <c r="I102" s="2"/>
-      <c r="J102" s="2" t="s">
-        <v>21</v>
-      </c>
+      <c r="J102" s="2"/>
     </row>
     <row r="103" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E103" s="3" t="s">
-        <v>59</v>
+        <v>36</v>
       </c>
       <c r="F103" s="9" t="s">
-        <v>15</v>
+        <v>37</v>
       </c>
       <c r="G103" s="10"/>
       <c r="H103" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="I103" s="2"/>
-      <c r="J103" s="2"/>
+      <c r="I103" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="J103" s="2" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="104" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E104" s="3" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="F104" s="9" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="G104" s="10"/>
       <c r="H104" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="I104" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="J104" s="2" t="s">
-        <v>48</v>
-      </c>
+      <c r="I104" s="2"/>
+      <c r="J104" s="2"/>
     </row>
     <row r="105" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E105" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="F105" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="G105" s="10"/>
+        <v>61</v>
+      </c>
+      <c r="F105" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="G105" s="10">
+        <v>8.1999999999999993</v>
+      </c>
       <c r="H105" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="I105" s="2"/>
-      <c r="J105" s="2"/>
+      <c r="I105" s="3"/>
+      <c r="J105" s="3"/>
     </row>
     <row r="106" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E106" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="F106" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="G106" s="10">
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="H106" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="I106" s="3"/>
-      <c r="J106" s="3"/>
+      <c r="E106" s="2"/>
+      <c r="F106" s="2"/>
+      <c r="G106" s="10"/>
+      <c r="H106" s="10"/>
+      <c r="I106" s="2"/>
+      <c r="J106" s="2"/>
     </row>
     <row r="107" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E107" s="2"/>
@@ -2095,24 +2087,16 @@
       <c r="I108" s="2"/>
       <c r="J108" s="2"/>
     </row>
-    <row r="109" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E109" s="2"/>
-      <c r="F109" s="2"/>
-      <c r="G109" s="10"/>
-      <c r="H109" s="10"/>
-      <c r="I109" s="2"/>
-      <c r="J109" s="2"/>
-    </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="E99:J99"/>
-    <mergeCell ref="E70:J70"/>
-    <mergeCell ref="E84:J84"/>
+    <mergeCell ref="E98:J98"/>
+    <mergeCell ref="E69:J69"/>
+    <mergeCell ref="E83:J83"/>
     <mergeCell ref="E3:J3"/>
     <mergeCell ref="E20:J20"/>
     <mergeCell ref="E34:J34"/>
-    <mergeCell ref="E46:J46"/>
-    <mergeCell ref="E56:J56"/>
+    <mergeCell ref="E45:J45"/>
+    <mergeCell ref="E55:J55"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>

<commit_message>
Se agregan trigger en tabla facturas y procedimientos en tabla empleados
</commit_message>
<xml_diff>
--- a/Etapa 01/Diccionario de datos.xlsx
+++ b/Etapa 01/Diccionario de datos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\INA\Proyecto Final\Etapa 01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB47D8A7-37F2-4795-ADA5-318770070868}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6F25318-B129-481C-B382-3CA09D089696}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-110" windowWidth="17020" windowHeight="10120" xr2:uid="{DA776B2A-F68D-4D43-820F-6C5204E56763}"/>
+    <workbookView xWindow="18980" yWindow="0" windowWidth="17020" windowHeight="10120" xr2:uid="{DA776B2A-F68D-4D43-820F-6C5204E56763}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
Se crean los procedimientos almacenado para las tablas empleados, proovedores, productos, facturas y se agrega el filtrado de busqueda por fecha y por empleado
</commit_message>
<xml_diff>
--- a/Etapa 01/Diccionario de datos.xlsx
+++ b/Etapa 01/Diccionario de datos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\INA\Proyecto Final\Etapa 01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6F25318-B129-481C-B382-3CA09D089696}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CC3F905-832D-4F09-B1C7-6B168B8AD3EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18980" yWindow="0" windowWidth="17020" windowHeight="10120" xr2:uid="{DA776B2A-F68D-4D43-820F-6C5204E56763}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DA776B2A-F68D-4D43-820F-6C5204E56763}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
Se realizan mejoras al planiamiento en general
</commit_message>
<xml_diff>
--- a/Etapa 01/Diccionario de datos.xlsx
+++ b/Etapa 01/Diccionario de datos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\INA\Proyecto Final\Etapa 01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CC3F905-832D-4F09-B1C7-6B168B8AD3EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FD52831-222B-4620-A05C-339BEEBE70FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DA776B2A-F68D-4D43-820F-6C5204E56763}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="67">
   <si>
     <t>Atributo</t>
   </si>
@@ -133,9 +133,6 @@
     <t>NOMBRE_PROVEEDOR</t>
   </si>
   <si>
-    <t>CODIGO_PRODUCTO</t>
-  </si>
-  <si>
     <t>Inventarios</t>
   </si>
   <si>
@@ -184,9 +181,6 @@
     <t xml:space="preserve">    &gt;= GETDATE()</t>
   </si>
   <si>
-    <t>CANTIDAD_SALIDA</t>
-  </si>
-  <si>
     <t>SUBTOTAL</t>
   </si>
   <si>
@@ -226,12 +220,6 @@
     <t>NUM_IDENTIFICACION</t>
   </si>
   <si>
-    <t>Detalle_Facturas</t>
-  </si>
-  <si>
-    <t>ID_DETALLE_FACTURA</t>
-  </si>
-  <si>
     <t>Productos</t>
   </si>
   <si>
@@ -239,6 +227,15 @@
   </si>
   <si>
     <t xml:space="preserve">INT </t>
+  </si>
+  <si>
+    <t>CANTIDAD_VENDIDA</t>
+  </si>
+  <si>
+    <t>CANTIDAD_INGRESADA</t>
+  </si>
+  <si>
+    <t>DESCUENTO</t>
   </si>
 </sst>
 </file>
@@ -324,7 +321,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
@@ -349,6 +346,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
@@ -678,10 +681,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3CAD0CD-A372-4142-AD31-8AE87056CD94}">
-  <dimension ref="E2:L108"/>
+  <dimension ref="E2:L93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E32" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F39" sqref="F39"/>
+    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="J61" sqref="J61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -702,14 +705,14 @@
       <c r="J2" s="2"/>
     </row>
     <row r="3" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E3" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15"/>
-      <c r="J3" s="15"/>
+      <c r="E3" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="17"/>
     </row>
     <row r="4" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E4" s="5" t="s">
@@ -733,7 +736,7 @@
     </row>
     <row r="5" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E5" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F5" s="7" t="s">
         <v>15</v>
@@ -815,7 +818,7 @@
     </row>
     <row r="10" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E10" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F10" s="9" t="s">
         <v>6</v>
@@ -824,7 +827,7 @@
         <v>20</v>
       </c>
       <c r="H10" s="9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
@@ -867,20 +870,20 @@
     </row>
     <row r="13" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E13" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G13" s="10"/>
       <c r="H13" s="9" t="s">
         <v>7</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="5:10" x14ac:dyDescent="0.25">
@@ -901,7 +904,7 @@
     </row>
     <row r="15" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E15" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F15" s="8" t="s">
         <v>6</v>
@@ -949,14 +952,14 @@
       <c r="J19" s="2"/>
     </row>
     <row r="20" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E20" s="14" t="s">
+      <c r="E20" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="F20" s="15"/>
-      <c r="G20" s="15"/>
-      <c r="H20" s="15"/>
-      <c r="I20" s="15"/>
-      <c r="J20" s="15"/>
+      <c r="F20" s="17"/>
+      <c r="G20" s="17"/>
+      <c r="H20" s="17"/>
+      <c r="I20" s="17"/>
+      <c r="J20" s="17"/>
     </row>
     <row r="21" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E21" s="5" t="s">
@@ -1023,7 +1026,7 @@
         <v>100</v>
       </c>
       <c r="H24" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
@@ -1053,14 +1056,14 @@
       </c>
       <c r="G26" s="5"/>
       <c r="H26" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I26" s="3"/>
       <c r="J26" s="3"/>
     </row>
     <row r="27" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E27" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F27" s="9" t="s">
         <v>6</v>
@@ -1069,7 +1072,7 @@
         <v>25</v>
       </c>
       <c r="H27" s="9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I27" s="3"/>
       <c r="J27" s="3"/>
@@ -1090,213 +1093,217 @@
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>
     </row>
-    <row r="29" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E29" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F29" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="G29" s="5">
+    <row r="31" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E31" s="11">
+        <v>3</v>
+      </c>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
+      <c r="I31" s="2"/>
+      <c r="J31" s="2"/>
+    </row>
+    <row r="32" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E32" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="F32" s="17"/>
+      <c r="G32" s="17"/>
+      <c r="H32" s="17"/>
+      <c r="I32" s="17"/>
+      <c r="J32" s="17"/>
+    </row>
+    <row r="33" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E33" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="G33" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H33" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="I33" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="J33" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E34" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F34" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G34" s="5">
         <v>50</v>
       </c>
-      <c r="H29" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="I29" s="4"/>
-      <c r="J29" s="2"/>
-    </row>
-    <row r="30" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E30" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F30" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="G30" s="5">
-        <v>100</v>
-      </c>
-      <c r="H30" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="I30" s="2"/>
-      <c r="J30" s="2"/>
-    </row>
-    <row r="33" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E33" s="11">
-        <v>3</v>
-      </c>
-      <c r="F33" s="2"/>
-      <c r="G33" s="2"/>
-      <c r="H33" s="2"/>
-      <c r="I33" s="2"/>
-      <c r="J33" s="2"/>
-    </row>
-    <row r="34" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E34" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="F34" s="15"/>
-      <c r="G34" s="15"/>
-      <c r="H34" s="15"/>
-      <c r="I34" s="15"/>
-      <c r="J34" s="15"/>
+      <c r="H34" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="I34" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J34" s="3" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="35" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E35" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="F35" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="G35" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="H35" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="I35" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="J35" s="5" t="s">
-        <v>5</v>
+      <c r="E35" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F35" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G35" s="5"/>
+      <c r="H35" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="I35" s="2"/>
+      <c r="J35" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="36" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E36" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="F36" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="G36" s="5"/>
-      <c r="H36" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="I36" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="J36" s="3" t="s">
-        <v>8</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="F36" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="G36" s="10">
+        <v>100</v>
+      </c>
+      <c r="H36" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="I36" s="2"/>
+      <c r="J36" s="2"/>
     </row>
     <row r="37" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E37" s="3" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="G37" s="5"/>
+        <v>23</v>
+      </c>
+      <c r="G37" s="5">
+        <v>8.1999999999999993</v>
+      </c>
       <c r="H37" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I37" s="2"/>
-      <c r="J37" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="38" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E38" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="F38" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="G38" s="10">
-        <v>50</v>
-      </c>
-      <c r="H38" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="I38" s="2"/>
-      <c r="J38" s="2"/>
-    </row>
-    <row r="39" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E39" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="F39" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="G39" s="10">
-        <v>100</v>
-      </c>
-      <c r="H39" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="I39" s="2"/>
-      <c r="J39" s="2"/>
+      <c r="I37" s="3"/>
+      <c r="J37" s="3"/>
     </row>
     <row r="40" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E40" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F40" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="G40" s="5"/>
-      <c r="H40" s="6" t="s">
-        <v>7</v>
-      </c>
+      <c r="E40" s="11">
+        <v>4</v>
+      </c>
+      <c r="F40" s="2"/>
+      <c r="G40" s="2"/>
+      <c r="H40" s="2"/>
       <c r="I40" s="2"/>
       <c r="J40" s="2"/>
     </row>
     <row r="41" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E41" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="F41" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="G41" s="5">
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="H41" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="I41" s="3"/>
-      <c r="J41" s="3"/>
+      <c r="E41" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="F41" s="17"/>
+      <c r="G41" s="17"/>
+      <c r="H41" s="17"/>
+      <c r="I41" s="17"/>
+      <c r="J41" s="17"/>
+    </row>
+    <row r="42" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E42" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="F42" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="G42" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="H42" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="I42" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J42" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E43" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F43" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G43" s="8"/>
+      <c r="H43" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I43" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J43" s="3" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="44" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E44" s="11">
-        <v>4</v>
-      </c>
-      <c r="F44" s="2"/>
-      <c r="G44" s="2"/>
-      <c r="H44" s="2"/>
+      <c r="E44" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F44" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G44" s="8"/>
+      <c r="H44" s="7" t="s">
+        <v>7</v>
+      </c>
       <c r="I44" s="2"/>
-      <c r="J44" s="2"/>
+      <c r="J44" s="2" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="45" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E45" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="F45" s="15"/>
-      <c r="G45" s="15"/>
-      <c r="H45" s="15"/>
-      <c r="I45" s="15"/>
-      <c r="J45" s="15"/>
+      <c r="E45" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F45" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G45" s="8">
+        <v>100</v>
+      </c>
+      <c r="H45" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I45" s="2"/>
+      <c r="J45" s="2"/>
     </row>
     <row r="46" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E46" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="F46" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="G46" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="H46" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="I46" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="J46" s="8" t="s">
-        <v>5</v>
-      </c>
+      <c r="E46" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="F46" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="G46" s="15"/>
+      <c r="H46" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="I46" s="2"/>
+      <c r="J46" s="2"/>
     </row>
     <row r="47" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E47" s="3" t="s">
@@ -1309,197 +1316,193 @@
       <c r="H47" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I47" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="J47" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="I47" s="3"/>
+      <c r="J47" s="3"/>
     </row>
     <row r="48" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E48" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="F48" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="F48" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="G48" s="8"/>
-      <c r="H48" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="I48" s="2"/>
-      <c r="J48" s="2" t="s">
-        <v>21</v>
-      </c>
+      <c r="G48" s="15"/>
+      <c r="H48" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="I48" s="3"/>
+      <c r="J48" s="3"/>
     </row>
     <row r="49" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E49" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="F49" s="7" t="s">
-        <v>6</v>
+      <c r="E49" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F49" s="8" t="s">
+        <v>23</v>
       </c>
       <c r="G49" s="8">
-        <v>100</v>
-      </c>
-      <c r="H49" s="7" t="s">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="H49" s="8" t="s">
         <v>7</v>
       </c>
       <c r="I49" s="2"/>
       <c r="J49" s="2"/>
     </row>
-    <row r="50" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E50" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="F50" s="7" t="s">
+    <row r="52" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E52" s="11">
+        <v>5</v>
+      </c>
+      <c r="F52" s="2"/>
+      <c r="G52" s="2"/>
+      <c r="H52" s="2"/>
+      <c r="I52" s="2"/>
+      <c r="J52" s="2"/>
+    </row>
+    <row r="53" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E53" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="F53" s="17"/>
+      <c r="G53" s="17"/>
+      <c r="H53" s="17"/>
+      <c r="I53" s="17"/>
+      <c r="J53" s="17"/>
+    </row>
+    <row r="54" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E54" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="F54" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="G54" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="H54" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="I54" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J54" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="55" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E55" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F55" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="G50" s="8"/>
-      <c r="H50" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="I50" s="3"/>
-      <c r="J50" s="3"/>
-    </row>
-    <row r="51" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E51" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="F51" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="G51" s="8">
-        <v>10.199999999999999</v>
-      </c>
-      <c r="H51" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="I51" s="2"/>
-      <c r="J51" s="2"/>
-    </row>
-    <row r="54" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E54" s="11">
-        <v>5</v>
-      </c>
-      <c r="F54" s="2"/>
-      <c r="G54" s="2"/>
-      <c r="H54" s="2"/>
-      <c r="I54" s="2"/>
-      <c r="J54" s="2"/>
-    </row>
-    <row r="55" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E55" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="F55" s="15"/>
-      <c r="G55" s="15"/>
-      <c r="H55" s="15"/>
-      <c r="I55" s="15"/>
-      <c r="J55" s="15"/>
+      <c r="G55" s="8"/>
+      <c r="H55" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I55" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J55" s="3" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="56" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E56" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="F56" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="G56" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="H56" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="I56" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="J56" s="8" t="s">
-        <v>5</v>
+      <c r="E56" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F56" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G56" s="8"/>
+      <c r="H56" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I56" s="2"/>
+      <c r="J56" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="57" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E57" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F57" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="G57" s="8"/>
+        <v>6</v>
+      </c>
+      <c r="G57" s="8">
+        <v>50</v>
+      </c>
       <c r="H57" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I57" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="J57" s="3" t="s">
-        <v>8</v>
+      <c r="I57" s="2"/>
+      <c r="J57" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="58" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E58" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F58" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G58" s="8">
+        <v>100</v>
+      </c>
+      <c r="H58" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I58" s="3"/>
+      <c r="J58" s="3"/>
+    </row>
+    <row r="59" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E59" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F59" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="G58" s="8"/>
-      <c r="H58" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="I58" s="2"/>
-      <c r="J58" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="59" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E59" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="F59" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="G59" s="8">
-        <v>50</v>
-      </c>
-      <c r="H59" s="7" t="s">
+      <c r="G59" s="8"/>
+      <c r="H59" s="8" t="s">
         <v>7</v>
       </c>
       <c r="I59" s="2"/>
-      <c r="J59" s="2" t="s">
-        <v>21</v>
-      </c>
+      <c r="J59" s="2"/>
+      <c r="L59" s="1"/>
     </row>
     <row r="60" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E60" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="F60" s="7" t="s">
-        <v>6</v>
+      <c r="E60" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F60" s="8" t="s">
+        <v>23</v>
       </c>
       <c r="G60" s="8">
-        <v>100</v>
-      </c>
-      <c r="H60" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="I60" s="3"/>
-      <c r="J60" s="3"/>
+        <v>10.199999999999999</v>
+      </c>
+      <c r="H60" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="I60" s="2"/>
+      <c r="J60" s="2"/>
     </row>
     <row r="61" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E61" s="2" t="s">
-        <v>22</v>
+        <v>48</v>
       </c>
       <c r="F61" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="G61" s="8"/>
+        <v>23</v>
+      </c>
+      <c r="G61" s="8">
+        <v>10.199999999999999</v>
+      </c>
       <c r="H61" s="8" t="s">
         <v>7</v>
       </c>
       <c r="I61" s="2"/>
       <c r="J61" s="2"/>
-      <c r="L61" s="1"/>
     </row>
     <row r="62" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E62" s="2" t="s">
@@ -1511,145 +1514,145 @@
       <c r="G62" s="8">
         <v>10.199999999999999</v>
       </c>
-      <c r="H62" s="8" t="s">
-        <v>7</v>
-      </c>
+      <c r="H62" s="8"/>
       <c r="I62" s="2"/>
       <c r="J62" s="2"/>
     </row>
     <row r="63" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E63" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F63" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="F63" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="G63" s="8">
+      <c r="G63" s="15">
         <v>10.199999999999999</v>
       </c>
-      <c r="H63" s="8" t="s">
-        <v>7</v>
-      </c>
+      <c r="H63" s="15"/>
       <c r="I63" s="2"/>
       <c r="J63" s="2"/>
     </row>
     <row r="64" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E64" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F64" s="8">
-        <v>4.2</v>
-      </c>
-      <c r="G64" s="8"/>
-      <c r="H64" s="8"/>
+        <v>59</v>
+      </c>
+      <c r="F64" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="G64" s="10">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="H64" s="10" t="s">
+        <v>7</v>
+      </c>
       <c r="I64" s="2"/>
       <c r="J64" s="2"/>
     </row>
-    <row r="65" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E65" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="F65" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="G65" s="10">
-        <v>10.199999999999999</v>
-      </c>
-      <c r="H65" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="I65" s="2"/>
-      <c r="J65" s="2"/>
+    <row r="67" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E67" s="11">
+        <v>6</v>
+      </c>
+      <c r="F67" s="2"/>
+      <c r="G67" s="2"/>
+      <c r="H67" s="2"/>
+      <c r="I67" s="2"/>
+      <c r="J67" s="2"/>
     </row>
     <row r="68" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E68" s="11">
-        <v>6</v>
-      </c>
-      <c r="F68" s="2"/>
-      <c r="G68" s="2"/>
-      <c r="H68" s="2"/>
-      <c r="I68" s="2"/>
-      <c r="J68" s="2"/>
+      <c r="E68" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="F68" s="17"/>
+      <c r="G68" s="17"/>
+      <c r="H68" s="17"/>
+      <c r="I68" s="17"/>
+      <c r="J68" s="17"/>
     </row>
     <row r="69" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E69" s="14" t="s">
+      <c r="E69" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="F69" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="G69" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="H69" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="I69" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J69" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="70" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E70" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F69" s="15"/>
-      <c r="G69" s="15"/>
-      <c r="H69" s="15"/>
-      <c r="I69" s="15"/>
-      <c r="J69" s="15"/>
-    </row>
-    <row r="70" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E70" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="F70" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="G70" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="H70" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="I70" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="J70" s="8" t="s">
-        <v>5</v>
+      <c r="F70" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G70" s="8"/>
+      <c r="H70" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I70" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J70" s="3" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="71" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E71" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="F71" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F71" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="G71" s="8"/>
-      <c r="H71" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="I71" s="3" t="s">
-        <v>16</v>
-      </c>
+      <c r="G71" s="13"/>
+      <c r="H71" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="I71" s="3"/>
       <c r="J71" s="3" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
     </row>
     <row r="72" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E72" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="F72" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="G72" s="13"/>
-      <c r="H72" s="12" t="s">
-        <v>7</v>
+        <v>60</v>
+      </c>
+      <c r="F72" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="G72" s="10">
+        <v>20</v>
+      </c>
+      <c r="H72" s="9" t="s">
+        <v>52</v>
       </c>
       <c r="I72" s="3"/>
-      <c r="J72" s="3" t="s">
-        <v>21</v>
-      </c>
+      <c r="J72" s="3"/>
     </row>
     <row r="73" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E73" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F73" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="G73" s="10">
+        <v>41</v>
+      </c>
+      <c r="F73" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G73" s="8">
         <v>20</v>
       </c>
-      <c r="H73" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="I73" s="3"/>
-      <c r="J73" s="3"/>
+      <c r="H73" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I73" s="2"/>
+      <c r="J73" s="2"/>
     </row>
     <row r="74" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E74" s="3" t="s">
@@ -1680,148 +1683,150 @@
       <c r="H75" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I75" s="2"/>
-      <c r="J75" s="2"/>
+      <c r="I75" s="3"/>
+      <c r="J75" s="3"/>
     </row>
     <row r="76" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E76" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="F76" s="7" t="s">
+      <c r="E76" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F76" s="8" t="s">
         <v>6</v>
       </c>
       <c r="G76" s="8">
         <v>20</v>
       </c>
-      <c r="H76" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="I76" s="3"/>
-      <c r="J76" s="3"/>
+      <c r="H76" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="I76" s="2"/>
+      <c r="J76" s="2"/>
     </row>
     <row r="77" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E77" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F77" s="8" t="s">
         <v>6</v>
       </c>
       <c r="G77" s="8">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="H77" s="8" t="s">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="I77" s="2"/>
       <c r="J77" s="2"/>
     </row>
     <row r="78" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E78" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F78" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="G78" s="8">
-        <v>100</v>
-      </c>
-      <c r="H78" s="8" t="s">
-        <v>54</v>
-      </c>
+      <c r="E78" s="2"/>
+      <c r="F78" s="2"/>
+      <c r="G78" s="8"/>
+      <c r="H78" s="8"/>
       <c r="I78" s="2"/>
       <c r="J78" s="2"/>
     </row>
-    <row r="79" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E79" s="2"/>
-      <c r="F79" s="2"/>
-      <c r="G79" s="8"/>
-      <c r="H79" s="8"/>
-      <c r="I79" s="2"/>
-      <c r="J79" s="2"/>
+    <row r="81" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E81" s="11">
+        <v>7</v>
+      </c>
+      <c r="F81" s="2"/>
+      <c r="G81" s="2"/>
+      <c r="H81" s="2"/>
+      <c r="I81" s="2"/>
+      <c r="J81" s="2"/>
     </row>
     <row r="82" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E82" s="11">
-        <v>7</v>
-      </c>
-      <c r="F82" s="2"/>
-      <c r="G82" s="2"/>
-      <c r="H82" s="2"/>
-      <c r="I82" s="2"/>
-      <c r="J82" s="2"/>
+      <c r="E82" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="F82" s="17"/>
+      <c r="G82" s="17"/>
+      <c r="H82" s="17"/>
+      <c r="I82" s="17"/>
+      <c r="J82" s="17"/>
     </row>
     <row r="83" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E83" s="14" t="s">
+      <c r="E83" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="F83" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="G83" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="H83" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="I83" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J83" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="84" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E84" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="F83" s="15"/>
-      <c r="G83" s="15"/>
-      <c r="H83" s="15"/>
-      <c r="I83" s="15"/>
-      <c r="J83" s="15"/>
-    </row>
-    <row r="84" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E84" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="F84" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="G84" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="H84" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="I84" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="J84" s="8" t="s">
-        <v>5</v>
+      <c r="F84" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G84" s="8"/>
+      <c r="H84" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I84" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J84" s="3" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="85" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E85" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="F85" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="G85" s="8"/>
-      <c r="H85" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="I85" s="3" t="s">
-        <v>16</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="F85" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="G85" s="13"/>
+      <c r="H85" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="I85" s="3"/>
       <c r="J85" s="3" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
     </row>
     <row r="86" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E86" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="F86" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="G86" s="13"/>
-      <c r="H86" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="I86" s="3"/>
-      <c r="J86" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F86" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G86" s="8"/>
+      <c r="H86" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I86" s="2"/>
+      <c r="J86" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="87" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E87" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="F87" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="G87" s="8"/>
-      <c r="H87" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="F87" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="G87" s="13">
+        <v>50</v>
+      </c>
+      <c r="H87" s="12" t="s">
         <v>7</v>
       </c>
       <c r="I87" s="2"/>
@@ -1831,83 +1836,73 @@
     </row>
     <row r="88" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E88" s="3" t="s">
-        <v>57</v>
+        <v>29</v>
       </c>
       <c r="F88" s="12" t="s">
         <v>6</v>
       </c>
       <c r="G88" s="13">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="H88" s="12" t="s">
         <v>7</v>
       </c>
       <c r="I88" s="2"/>
-      <c r="J88" s="2" t="s">
-        <v>21</v>
-      </c>
+      <c r="J88" s="2"/>
     </row>
     <row r="89" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E89" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="F89" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="G89" s="13">
-        <v>100</v>
-      </c>
-      <c r="H89" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="I89" s="2"/>
-      <c r="J89" s="2"/>
+        <v>35</v>
+      </c>
+      <c r="F89" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="G89" s="8"/>
+      <c r="H89" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I89" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J89" s="2" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="90" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E90" s="3" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="F90" s="7" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="G90" s="8"/>
       <c r="H90" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I90" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="J90" s="2" t="s">
-        <v>48</v>
-      </c>
+      <c r="I90" s="2"/>
+      <c r="J90" s="2"/>
     </row>
     <row r="91" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E91" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F91" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="G91" s="8"/>
-      <c r="H91" s="7" t="s">
+      <c r="E91" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F91" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="G91" s="8">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="H91" s="8" t="s">
         <v>7</v>
       </c>
       <c r="I91" s="2"/>
       <c r="J91" s="2"/>
     </row>
     <row r="92" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E92" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="F92" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="G92" s="8">
-        <v>10.199999999999999</v>
-      </c>
-      <c r="H92" s="8" t="s">
-        <v>7</v>
-      </c>
+      <c r="E92" s="2"/>
+      <c r="F92" s="2"/>
+      <c r="G92" s="8"/>
+      <c r="H92" s="8"/>
       <c r="I92" s="2"/>
       <c r="J92" s="2"/>
     </row>
@@ -1919,184 +1914,15 @@
       <c r="I93" s="2"/>
       <c r="J93" s="2"/>
     </row>
-    <row r="94" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E94" s="2"/>
-      <c r="F94" s="2"/>
-      <c r="G94" s="8"/>
-      <c r="H94" s="8"/>
-      <c r="I94" s="2"/>
-      <c r="J94" s="2"/>
-    </row>
-    <row r="97" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E97" s="11">
-        <v>8</v>
-      </c>
-      <c r="F97" s="2"/>
-      <c r="G97" s="2"/>
-      <c r="H97" s="2"/>
-      <c r="I97" s="2"/>
-      <c r="J97" s="2"/>
-    </row>
-    <row r="98" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E98" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="F98" s="15"/>
-      <c r="G98" s="15"/>
-      <c r="H98" s="15"/>
-      <c r="I98" s="15"/>
-      <c r="J98" s="15"/>
-    </row>
-    <row r="99" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E99" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="F99" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="G99" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="H99" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="I99" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="J99" s="10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="100" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E100" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="F100" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="G100" s="10"/>
-      <c r="H100" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="I100" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="J100" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="101" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E101" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="F101" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="G101" s="10"/>
-      <c r="H101" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="I101" s="2"/>
-      <c r="J101" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="102" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E102" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="F102" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="G102" s="10"/>
-      <c r="H102" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="I102" s="2"/>
-      <c r="J102" s="2"/>
-    </row>
-    <row r="103" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E103" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="F103" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="G103" s="10"/>
-      <c r="H103" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="I103" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="J103" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="104" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E104" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="F104" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="G104" s="10"/>
-      <c r="H104" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="I104" s="2"/>
-      <c r="J104" s="2"/>
-    </row>
-    <row r="105" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E105" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="F105" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="G105" s="10">
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="H105" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="I105" s="3"/>
-      <c r="J105" s="3"/>
-    </row>
-    <row r="106" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E106" s="2"/>
-      <c r="F106" s="2"/>
-      <c r="G106" s="10"/>
-      <c r="H106" s="10"/>
-      <c r="I106" s="2"/>
-      <c r="J106" s="2"/>
-    </row>
-    <row r="107" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E107" s="2"/>
-      <c r="F107" s="2"/>
-      <c r="G107" s="10"/>
-      <c r="H107" s="10"/>
-      <c r="I107" s="2"/>
-      <c r="J107" s="2"/>
-    </row>
-    <row r="108" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E108" s="2"/>
-      <c r="F108" s="2"/>
-      <c r="G108" s="10"/>
-      <c r="H108" s="10"/>
-      <c r="I108" s="2"/>
-      <c r="J108" s="2"/>
-    </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="E98:J98"/>
-    <mergeCell ref="E69:J69"/>
-    <mergeCell ref="E83:J83"/>
+  <mergeCells count="7">
+    <mergeCell ref="E68:J68"/>
+    <mergeCell ref="E82:J82"/>
     <mergeCell ref="E3:J3"/>
     <mergeCell ref="E20:J20"/>
-    <mergeCell ref="E34:J34"/>
-    <mergeCell ref="E45:J45"/>
-    <mergeCell ref="E55:J55"/>
+    <mergeCell ref="E32:J32"/>
+    <mergeCell ref="E41:J41"/>
+    <mergeCell ref="E53:J53"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>